<commit_message>
Added some new words and its meaning and bangla meaning
</commit_message>
<xml_diff>
--- a/Vocabulary/vocabu.xlsx
+++ b/Vocabulary/vocabu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
   <si>
     <t>Word</t>
   </si>
@@ -211,6 +211,100 @@
   </si>
   <si>
     <t>they were agreeable to its publication</t>
+  </si>
+  <si>
+    <t>hypotheses</t>
+  </si>
+  <si>
+    <t>guess, supposition, inference</t>
+  </si>
+  <si>
+    <t>colleague,partner, cooperator</t>
+  </si>
+  <si>
+    <t>have in common with</t>
+  </si>
+  <si>
+    <t>likeness, take after</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ভক্তি
+</t>
+  </si>
+  <si>
+    <t>piety, worship, adoration</t>
+  </si>
+  <si>
+    <t>prominent,distinguised, noted</t>
+  </si>
+  <si>
+    <t xml:space="preserve">মস্তকবিশিষ্ট
+</t>
+  </si>
+  <si>
+    <t>সিনকোনা গাছের ছাল থেকে প্রাপ্ত উপক্ষার</t>
+  </si>
+  <si>
+    <t>দিগন্ত</t>
+  </si>
+  <si>
+    <t>skyline, azimuth</t>
+  </si>
+  <si>
+    <t>erase,efface,mob,swob</t>
+  </si>
+  <si>
+    <t>আশাবাদ</t>
+  </si>
+  <si>
+    <t>হুমড়ি</t>
+  </si>
+  <si>
+    <t>peck, nibbling, pecking, reprimand</t>
+  </si>
+  <si>
+    <t>প্রত্যাশা</t>
+  </si>
+  <si>
+    <t>hope, expectation, prospect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">খসড়া
+</t>
+  </si>
+  <si>
+    <t>checkers, draughts</t>
+  </si>
+  <si>
+    <t>উচ্চতর</t>
+  </si>
+  <si>
+    <t>upper,best,excellent,beneficial</t>
+  </si>
+  <si>
+    <t>লক্ষণীয়</t>
+  </si>
+  <si>
+    <t>noticeable, remarkable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">জ্যোতির্বিদ্যা-সংক্রান্ত
+</t>
+  </si>
+  <si>
+    <t>scepticism</t>
+  </si>
+  <si>
+    <t>সংশয়বাদ</t>
+  </si>
+  <si>
+    <t>অনুরূপ</t>
+  </si>
+  <si>
+    <t>likeness</t>
+  </si>
+  <si>
+    <t>ক্ষয়িত</t>
   </si>
 </sst>
 </file>
@@ -246,8 +340,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,18 +625,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.85546875" customWidth="1"/>
+    <col min="4" max="4" width="41.28515625" customWidth="1"/>
     <col min="5" max="5" width="34.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -647,214 +744,308 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>79</v>
+      </c>
+      <c r="D21" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D27" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>75</v>
+      </c>
+      <c r="D39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>68</v>
+      </c>
+      <c r="D43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>87</v>
+      </c>
+      <c r="D47" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D50" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="D52" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>85</v>
+      </c>
+      <c r="D55" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>83</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>81</v>
+      </c>
+      <c r="D57" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>46</v>
+      </c>
+      <c r="C58" t="s">
+        <v>92</v>
+      </c>
+      <c r="D58" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>64</v>
+      </c>
+      <c r="C59" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>89</v>
+      </c>
+      <c r="D60" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added all the folder and resource for the vocabulary app
</commit_message>
<xml_diff>
--- a/Vocabulary/vocabu.xlsx
+++ b/Vocabulary/vocabu.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="2790" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>